<commit_message>
Se saca info de iibb para percepciones de la tabla clientes, se comienzan a ajustar algunas consultas de cc de proveedores relacionadas con factuas, pagos y balance de cuenta
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Tarea</t>
   </si>
@@ -25,6 +25,24 @@
   </si>
   <si>
     <t>calcular percepcion iibb en facturacion según parametro</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>no comenzado</t>
+  </si>
+  <si>
+    <t>en proceso</t>
+  </si>
+  <si>
+    <t>terminado</t>
+  </si>
+  <si>
+    <t>borrar de frontend y backend datos de percepcion</t>
+  </si>
+  <si>
+    <t>ajustar consultas de cc proveedores listado de fc y de pagos y balance de cuenta</t>
   </si>
 </sst>
 </file>
@@ -66,7 +84,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -363,45 +403,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="53.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"terminado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"en proceso"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"no comenzado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Hoja2!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Se realizan cambios en formularios para poder introducir descripciones manuales en codigos ZZZ, se comienza la creacion del rerporte historico de movimientos de articulos que incluye movimientos de stock y remitos
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Tarea</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>ajustar consultas de cc proveedores listado de fc y de pagos y balance de cuenta</t>
+  </si>
+  <si>
+    <t>revisar formularios y permitir ingreso de codigo ZZZ</t>
+  </si>
+  <si>
+    <t>crear formulario para cargar parametros del sistema</t>
+  </si>
+  <si>
+    <t>las consultas funcionan y mientras sigan asi no se ajustaran</t>
+  </si>
+  <si>
+    <t>generar reporte de historico de movimientos de articulos</t>
   </si>
 </sst>
 </file>
@@ -403,19 +415,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.140625" customWidth="1"/>
+    <col min="1" max="1" width="72.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,7 +436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -431,7 +444,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -439,7 +452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -447,11 +460,38 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Comienzo de tabla de parametros
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -418,7 +418,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -492,7 +492,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se termina formulario de parametros, se comienza reporte de mov. bancarios
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Tarea</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>generar reporte de historico de movimientos de articulos</t>
+  </si>
+  <si>
+    <t>terminar circuito de movimiento de bancos</t>
+  </si>
+  <si>
+    <t>generar reporte de mov de bancos</t>
+  </si>
+  <si>
+    <t>revisar reporte orden de pago esta fallando</t>
   </si>
 </sst>
 </file>
@@ -415,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,7 +493,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -493,6 +502,30 @@
       </c>
       <c r="B8" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios para cerrar circuito de movimientos bancarios con pagos a proveedores
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Tarea</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>revisar reporte orden de pago esta fallando</t>
+  </si>
+  <si>
+    <t>en reporte de OT resaltar observaciones</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,6 +528,14 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modificaciones a circuito de bancos, pagos y cobranzas
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Tarea</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>en reporte de OT resaltar observaciones</t>
+  </si>
+  <si>
+    <t>mejorar formulario de bancos para agregar cuenta bancaria</t>
+  </si>
+  <si>
+    <t>proveedores pagos, arreglar calculo de retenciones</t>
   </si>
 </sst>
 </file>
@@ -112,7 +118,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -126,7 +132,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -427,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +531,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
@@ -533,22 +539,38 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"terminado"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"no comenzado"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"en proceso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"no comenzado"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"terminado"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se terminan modificaciones de cobranzas y pagos para asociar las cuentas bancarias y se modifica reporte de OT por sector agrupando el estado de las ordenes
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Tarea</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>proveedores pagos, arreglar calculo de retenciones</t>
+  </si>
+  <si>
+    <t>reporte ot por sector , agregar filtro por estados agregar columna de cantidad y NC</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,6 +561,14 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se termina reporte de mov. de bancos, se agregar facturacion en dolares
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Tarea</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>reporte ot por sector , agregar filtro por estados agregar columna de cantidad y NC</t>
+  </si>
+  <si>
+    <t>cuando se anula una OT consultar si se quieren anular la OT asociadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facturacion en dolares </t>
   </si>
 </sst>
 </file>
@@ -436,15 +442,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -521,7 +527,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -529,7 +535,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -537,7 +543,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -545,7 +551,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -569,7 +575,23 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
posibilidad de modificar cantidades en OTS y cambios en reportes de ventas y OTs en general
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Tarea</t>
   </si>
@@ -82,6 +82,15 @@
   </si>
   <si>
     <t xml:space="preserve">facturacion en dolares </t>
+  </si>
+  <si>
+    <t>modificar en reportes de produccion filtrar ordenes anuladas</t>
+  </si>
+  <si>
+    <t>reportes de ventas, fcs en dolares multiplicar por TC</t>
+  </si>
+  <si>
+    <t>permitir modificaciond e cantidades en ots</t>
   </si>
 </sst>
 </file>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +592,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -591,6 +600,30 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mejora formulario de cuentas bancarias, desarrllo de funcion para relacionar ordenes a la inversa, correccion de anulacion de ordenes relacionadas
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Tarea</t>
   </si>
@@ -91,6 +91,21 @@
   </si>
   <si>
     <t>permitir modificaciond e cantidades en ots</t>
+  </si>
+  <si>
+    <t>implementar funcionalidad de atajos al servidor en tabla de articulos</t>
+  </si>
+  <si>
+    <t>aun no viable</t>
+  </si>
+  <si>
+    <t>analizar implementacion de cash flow</t>
+  </si>
+  <si>
+    <t>relacionar ordenes a la inversa</t>
+  </si>
+  <si>
+    <t>EN BUSQUEDA DE ART. CUANDO HACES CLICK EN DESCRIPCION SALTAR PARA TIPEAR AUTOMATICAMENTE</t>
   </si>
 </sst>
 </file>
@@ -451,15 +466,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="95.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -595,7 +610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -603,7 +618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -611,7 +626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -619,12 +634,47 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajuste OT recursiva inversa
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>Tarea</t>
   </si>
@@ -102,10 +102,13 @@
     <t>analizar implementacion de cash flow</t>
   </si>
   <si>
-    <t>relacionar ordenes a la inversa</t>
-  </si>
-  <si>
     <t>EN BUSQUEDA DE ART. CUANDO HACES CLICK EN DESCRIPCION SALTAR PARA TIPEAR AUTOMATICAMENTE</t>
+  </si>
+  <si>
+    <t>sistematizar el RG 14</t>
+  </si>
+  <si>
+    <t>relacionar ordenes a la inversa, revisar porque hacia abajo trae 2 veces el mismo item</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,17 +666,25 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios cuentas bancarias se puede eliminar logicamente
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Tarea</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>88706 al 88760 identificar</t>
+  </si>
+  <si>
+    <t>FORMULARIO DE BANCOS IMPLEMENTAR BAJA LOGICA JUNTO CON CUENTAS</t>
+  </si>
+  <si>
+    <t>agregar en seguimiento de OT el estado del OT buscada</t>
   </si>
 </sst>
 </file>
@@ -472,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,10 +694,26 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se termina reporte de saldo deudor, se mojora interfaz de seguimiento de OT
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>Tarea</t>
   </si>
@@ -117,7 +117,10 @@
     <t>FORMULARIO DE BANCOS IMPLEMENTAR BAJA LOGICA JUNTO CON CUENTAS</t>
   </si>
   <si>
-    <t>agregar en seguimiento de OT el estado del OT buscada</t>
+    <t>agregar en seguimiento de OT el estado del OT buscada y posibilidad de imprimir</t>
+  </si>
+  <si>
+    <t>implementar en tabla cobranza el importe total de la cobranza y terminar reporte de saldo deudor</t>
   </si>
 </sst>
 </file>
@@ -478,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,6 +717,14 @@
       </c>
       <c r="B27" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se identifican numeros correlativos de radiadores supersupestos
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>Tarea</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>implementar en tabla cobranza el importe total de la cobranza y terminar reporte de saldo deudor</t>
+  </si>
+  <si>
+    <t>no se aplica</t>
   </si>
 </sst>
 </file>
@@ -483,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +601,10 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -606,7 +612,7 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -697,7 +703,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
         <v>31</v>
@@ -708,7 +714,7 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -716,7 +722,7 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,7 +730,7 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se terminan detalles de CC clientes
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>Tarea</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>reporte de cobranzas corregir subreporte de liquidacion</t>
+  </si>
+  <si>
+    <t>balance en cc clientes, agregar a la entidad factura el campo de observacines</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,6 +767,14 @@
       </c>
       <c r="B31" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se suma la percepcion de IIBB al total de la FC
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>Tarea</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>balance en cc clientes, agregar a la entidad factura el campo de observacines</t>
+  </si>
+  <si>
+    <t>desarrollar num correlativa RG-010</t>
   </si>
 </sst>
 </file>
@@ -496,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,6 +777,14 @@
         <v>39</v>
       </c>
       <c r="B32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se corrige reporte de factura, remitos. Se reescriben consultas de CC de clientes y proveedores
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
+    <workbookView xWindow="240" yWindow="405" windowWidth="14805" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>Tarea</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>desarrollar num correlativa RG-010</t>
+  </si>
+  <si>
+    <t>facturacion de remitos pendientes en dolares esta fallando</t>
+  </si>
+  <si>
+    <t>balance en cc proveedores esta fallando</t>
   </si>
 </sst>
 </file>
@@ -499,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,6 +792,22 @@
       </c>
       <c r="B33" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Borrado logico de proveedores
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
   <si>
     <t>Tarea</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>balance en cc proveedores esta fallando</t>
+  </si>
+  <si>
+    <t>importar tabla articulos con precios y costos en moneda adecuada</t>
   </si>
 </sst>
 </file>
@@ -505,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +778,7 @@
         <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -808,6 +811,14 @@
       </c>
       <c r="B35" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios consulta de CC
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
   <si>
     <t>Tarea</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>importar tabla articulos con precios y costos en moneda adecuada</t>
+  </si>
+  <si>
+    <t>REPORTE DE COBRANZAS NO SE VISUALIZA EL TOTAL</t>
   </si>
 </sst>
 </file>
@@ -508,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,6 +821,14 @@
         <v>43</v>
       </c>
       <c r="B36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregar descuento fijo a clientes
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -514,7 +514,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +821,7 @@
         <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reporte de comprobantes no pagados, se valoriza el reporte de articulos pedidos
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
   <si>
     <t>Tarea</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>REPORTE DE COBRANZAS NO SE VISUALIZA EL TOTAL</t>
+  </si>
+  <si>
+    <t>reporte de comprobantes pagados</t>
+  </si>
+  <si>
+    <t>revisar cobranzas no imputadas a ningun comprobante</t>
   </si>
 </sst>
 </file>
@@ -511,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,6 +836,22 @@
       </c>
       <c r="B37" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reporte de inventario de cheques de terceros, correcion de msj de error para facturacion
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="54">
   <si>
     <t>Tarea</t>
   </si>
@@ -157,6 +157,27 @@
   </si>
   <si>
     <t>revisar cobranzas no imputadas a ningun comprobante</t>
+  </si>
+  <si>
+    <t>CARTEL CON N° DE REMITO A IMPIRIMIR ANTES DE GUARDAR</t>
+  </si>
+  <si>
+    <t>en fc agregar tipo de cambio al pie si alguno de los items tiene precio en dolares y se facturo en pesos</t>
+  </si>
+  <si>
+    <t>permitir campo decimal al hacer ingreso de materiales en modulo stock</t>
+  </si>
+  <si>
+    <t>permitir ingreso de pedidos tipo repuestos</t>
+  </si>
+  <si>
+    <t>facturacion cuando el cliente no tiene cargado prov y localidad tirrar el error adecuadoi</t>
+  </si>
+  <si>
+    <t>reporte inventario de cheque de terceros</t>
+  </si>
+  <si>
+    <t>ver maejo de error de facturacion AFIP</t>
   </si>
 </sst>
 </file>
@@ -198,7 +219,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -517,15 +580,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.7109375" customWidth="1"/>
+    <col min="1" max="1" width="95.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -843,7 +906,7 @@
         <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -854,15 +917,71 @@
         <v>4</v>
       </c>
     </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"no comenzado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"en proceso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"terminado"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
notas de debito sin IVA
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -219,49 +219,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -583,7 +541,7 @@
   <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,18 +928,18 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"no comenzado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"en proceso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"terminado"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
codigo de barras en factura con digito verificador
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="60">
   <si>
     <t>Tarea</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>facturacion generar codigo de validacion</t>
+  </si>
+  <si>
+    <t>frontend form articulos el codigo solo en mayusculas</t>
   </si>
 </sst>
 </file>
@@ -557,10 +560,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,6 +990,14 @@
         <v>58</v>
       </c>
       <c r="B51" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correccion reporte iva ventas restar nc
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
   <si>
     <t>Tarea</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>agregar localidad a form de remito</t>
+  </si>
+  <si>
+    <t>agregar campo peso a la tabla de articulos</t>
   </si>
 </sst>
 </file>
@@ -563,10 +566,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,6 +1012,14 @@
         <v>60</v>
       </c>
       <c r="B53" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correccion pago a proveedores tipo de pago cheque de terceros
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
   <si>
     <t>Tarea</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>agregar campo peso a la tabla de articulos</t>
+  </si>
+  <si>
+    <t>agregar filto a frontend de remitos</t>
   </si>
 </sst>
 </file>
@@ -566,10 +569,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A56" sqref="A55:A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,6 +1023,14 @@
         <v>61</v>
       </c>
       <c r="B54" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correccion anulacion de ots
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -572,7 +572,7 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A56" sqref="A55:A56"/>
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +991,7 @@
         <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -999,7 +999,7 @@
         <v>58</v>
       </c>
       <c r="B51" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1015,7 +1015,7 @@
         <v>60</v>
       </c>
       <c r="B53" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se separa campo nombre en apellido y nombre de personal
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
   <si>
     <t>Tarea</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>agregar filto a frontend de remitos</t>
+  </si>
+  <si>
+    <t>anular remito pendiente de fc</t>
   </si>
 </sst>
 </file>
@@ -569,10 +572,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,6 +1034,14 @@
         <v>62</v>
       </c>
       <c r="B55" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>63</v>
+      </c>
+      <c r="B56" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cc clientes, fc en dolares pasa a la cuenta en pesos segun el tc
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
   <si>
     <t>Tarea</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>anular remito pendiente de fc</t>
+  </si>
+  <si>
+    <t>facturacion, cambiar de precio solo los articulos en dolares con t/c</t>
   </si>
 </sst>
 </file>
@@ -572,10 +575,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,6 +1045,14 @@
         <v>63</v>
       </c>
       <c r="B56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>64</v>
+      </c>
+      <c r="B57" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
manejo de excepciones de facturacion
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="66">
   <si>
     <t>Tarea</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>facturacion, cambiar de precio solo los articulos en dolares con t/c</t>
+  </si>
+  <si>
+    <t>FILTRAR REMITO PENDIENTE DE FC X CLIENTE</t>
   </si>
 </sst>
 </file>
@@ -575,10 +578,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1048,7 @@
         <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1053,6 +1056,14 @@
         <v>64</v>
       </c>
       <c r="B57" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B58" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cambios en reporte recibos
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
   <si>
     <t>Tarea</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>FILTRAR REMITO PENDIENTE DE FC X CLIENTE</t>
+  </si>
+  <si>
+    <t>corregir generacion de recibos reporte</t>
   </si>
 </sst>
 </file>
@@ -578,10 +581,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,6 +1067,14 @@
         <v>65</v>
       </c>
       <c r="B58" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FILTRAR REMITO PENDIENTE DE FC X CLIENTE
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -583,8 +583,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1059,7 @@
         <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1067,7 +1067,7 @@
         <v>65</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
frontend form articulos el codigo solo en mayusculas
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -583,8 +583,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,7 +1003,7 @@
         <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1019,7 +1019,7 @@
         <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1043,7 +1043,7 @@
         <v>62</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
agregar campo peso a la tabla de articulos
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
   <si>
     <t>Tarea</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>corregir generacion de recibos reporte</t>
+  </si>
+  <si>
+    <t>agregar boton de estructura en tabla de articulos</t>
   </si>
 </sst>
 </file>
@@ -581,10 +584,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,6 +1078,14 @@
         <v>66</v>
       </c>
       <c r="B59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajustes a pedidos internos de materiales
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$60</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -586,8 +586,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,12 +760,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>25</v>
@@ -830,7 +830,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -865,12 +865,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -953,12 +953,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>51</v>
       </c>
       <c r="B44" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -969,7 +969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -977,7 +977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>58</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -1033,15 +1033,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>61</v>
       </c>
       <c r="B54" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>65</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>66</v>
       </c>
@@ -1090,10 +1090,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C47">
+  <autoFilter ref="A1:C60">
     <filterColumn colId="1">
       <filters>
-        <filter val="en proceso"/>
         <filter val="no comenzado"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
certificado de retencion segun res AGIP 382
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
   <si>
     <t>Tarea</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>percepciones txt percepciones pagadas</t>
+  </si>
+  <si>
+    <t>reportes de ot no estan funcionando</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -593,10 +617,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,15 +1126,32 @@
       <c r="A61" t="s">
         <v>68</v>
       </c>
+      <c r="B61" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>69</v>
       </c>
+      <c r="B62" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>70</v>
+      </c>
+      <c r="B63" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1122,13 +1163,13 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"no comenzado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"en proceso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"terminado"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
se ordena libro sueldos por apellido
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
   <si>
     <t>Tarea</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>reporte pedidos discriminar por respuestos</t>
+  </si>
+  <si>
+    <t>sacar codigo zzz del campo codigo de factura y remito</t>
   </si>
 </sst>
 </file>
@@ -602,10 +605,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,6 +1155,14 @@
         <v>73</v>
       </c>
       <c r="B66" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cambio de estructura frontend, implementacion TXT percepciones y retenciones
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="76">
   <si>
     <t>Tarea</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>sacar codigo zzz del campo codigo de factura y remito</t>
+  </si>
+  <si>
+    <t>resumen de cc prov y cliente</t>
   </si>
 </sst>
 </file>
@@ -285,7 +288,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -605,10 +629,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,7 +1139,7 @@
         <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1123,7 +1147,7 @@
         <v>69</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1131,7 +1155,7 @@
         <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1155,7 +1179,7 @@
         <v>73</v>
       </c>
       <c r="B66" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1163,6 +1187,14 @@
         <v>74</v>
       </c>
       <c r="B67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1175,13 +1207,13 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"no comenzado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"en proceso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"terminado"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
ordenes de compra y estructura de materiales
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -616,8 +616,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,7 +972,7 @@
         <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1028,7 +1028,7 @@
         <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1124,7 +1124,7 @@
         <v>68</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1140,7 +1140,7 @@
         <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1148,7 +1148,7 @@
         <v>71</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1180,7 +1180,7 @@
         <v>75</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
         <v>76</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1196,7 +1196,7 @@
         <v>77</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios en proxy para alta de clientes
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
   <si>
     <t>Tarea</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>grilla de pedidos internos y de tabla busqueda articulos hacerlas editables para seleccionar</t>
+  </si>
+  <si>
+    <t>AGREGAR EN CC PROV Y CLIENTES CAMPO PARA ANOTACIONES</t>
   </si>
 </sst>
 </file>
@@ -614,10 +617,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,6 +1200,14 @@
       </c>
       <c r="B70" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>78</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega archivo .gitignore para no contemplar los recursos de las carpetas public
Esta modificacion evitará tener que hacer commit de los recursos generados por el usuario tales como
documentos PDF, reportes, Excel, etc.
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="80">
   <si>
     <t>Tarea</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>AGREGAR EN CC PROV Y CLIENTES CAMPO PARA ANOTACIONES</t>
+  </si>
+  <si>
+    <t>ingreso de materiales, implementar grilla para tildar piezas controladas</t>
   </si>
 </sst>
 </file>
@@ -617,10 +620,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,6 +1211,14 @@
       </c>
       <c r="B71" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modulo para control de recepcion de materiales
Se implementa una grilla para que control de calidad verifique el ingreso de materiales
y pueda asignar num de certificado de calidad y asociar no conformidades.
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="81">
   <si>
     <t>Tarea</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>ingreso de materiales, implementar grilla para tildar piezas controladas</t>
+  </si>
+  <si>
+    <t>refrescar grilla de bancos cuando se guarda un movimiento</t>
   </si>
 </sst>
 </file>
@@ -620,9 +623,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
@@ -1218,6 +1221,14 @@
         <v>79</v>
       </c>
       <c r="B72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cuentas corrientes store procedure
Se borran las consultas SQL de CC y se reemplazan por procedimientos almacenados,
tanto para proveedores como para cliente.
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$74</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="84">
   <si>
     <t>Tarea</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>buscar proveedores y cliente por CUIT, en bd campo cuit unico</t>
+  </si>
+  <si>
+    <t>CC CLIENTES ORDENAR POR FECHA</t>
+  </si>
+  <si>
+    <t>CC PROVEEDORES PINTAR FILAS PAGADAS</t>
   </si>
 </sst>
 </file>
@@ -306,7 +312,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -626,10 +653,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,15 +1238,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>79</v>
       </c>
@@ -1227,7 +1254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>80</v>
       </c>
@@ -1243,8 +1270,24 @@
         <v>4</v>
       </c>
     </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C71">
+  <autoFilter ref="A1:C74">
     <filterColumn colId="1">
       <filters>
         <filter val="en proceso"/>
@@ -1253,13 +1296,13 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"no comenzado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"en proceso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"terminado"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Cambios reporte estructura de materiales
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="85">
   <si>
     <t>Tarea</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>CC PROVEEDORES PINTAR FILAS PAGADAS</t>
+  </si>
+  <si>
+    <t>comisiones por vendedor</t>
   </si>
 </sst>
 </file>
@@ -312,28 +315,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -653,10 +635,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,6 +1268,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>84</v>
+      </c>
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C74">
     <filterColumn colId="1">
@@ -1296,13 +1286,13 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"no comenzado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"en proceso"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"terminado"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix retenciones de IIBB
Se ajusta el calculo de rentenciones de IIBB para aquellas facturas con un neto mayor a el parametro de tope en este caso 2000
pesos a la fecha 17-5-18
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="87">
   <si>
     <t>Tarea</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>comisiones por vendedor</t>
+  </si>
+  <si>
+    <t>cc ordenar tambien por numero de fc para las fcs q estan en la misma fehca</t>
+  </si>
+  <si>
+    <t>ver calculo de total en reporte de comisiones</t>
   </si>
 </sst>
 </file>
@@ -635,10 +641,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,6 +1280,22 @@
       </c>
       <c r="B77" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix retenciones IIBB TXT
Se modifica la consulta de los TXT
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="88">
   <si>
     <t>Tarea</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>ver calculo de total en reporte de comisiones</t>
+  </si>
+  <si>
+    <t>pedidos internos de compras sacar grilla zebra</t>
   </si>
 </sst>
 </file>
@@ -641,10 +644,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,7 +1266,7 @@
         <v>82</v>
       </c>
       <c r="B75" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1287,7 +1290,7 @@
         <v>85</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1295,6 +1298,14 @@
         <v>86</v>
       </c>
       <c r="B79" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correccion reporte IVA ventas
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="89">
   <si>
     <t>Tarea</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>pedidos internos de compras sacar grilla zebra</t>
+  </si>
+  <si>
+    <t>ver sumatoria reporte resumen saldo deudor</t>
   </si>
 </sst>
 </file>
@@ -644,10 +647,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1165,7 @@
         <v>69</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1210,7 +1213,7 @@
         <v>75</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1306,6 +1309,14 @@
         <v>87</v>
       </c>
       <c r="B80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix reporte estructura de materiales segun estrategia closure
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="89">
   <si>
     <t>Tarea</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>pedidos internos de compras sacar grilla zebra</t>
+  </si>
+  <si>
+    <t>pedidos a compras internos cargar cantidad con coma</t>
   </si>
 </sst>
 </file>
@@ -644,10 +647,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1306,6 +1309,14 @@
         <v>87</v>
       </c>
       <c r="B80" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>88</v>
+      </c>
+      <c r="B81" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se modifica la estrategia de formulas a closure
Se implementa en fase de produccion la nueva estrategia de formulas.
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$82</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="90">
   <si>
     <t>Tarea</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>ver sumatoria reporte resumen saldo deudor</t>
+  </si>
+  <si>
+    <t>cotizaciones corregir descuentos</t>
   </si>
 </sst>
 </file>
@@ -647,10 +650,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,7 +1163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -1208,7 +1211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>75</v>
       </c>
@@ -1264,7 +1267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>82</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>85</v>
       </c>
@@ -1320,8 +1323,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C74">
+  <autoFilter ref="A1:C82">
     <filterColumn colId="1">
       <filters>
         <filter val="en proceso"/>

</xml_diff>

<commit_message>
Busqueda de clientes y proveedores por cuit
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="91">
   <si>
     <t>Tarea</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>cotizaciones corregir descuentos</t>
+  </si>
+  <si>
+    <t>costos de articulos calcular aquellos q estan formulados</t>
   </si>
 </sst>
 </file>
@@ -650,10 +653,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,7 +1267,7 @@
         <v>81</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1329,6 +1332,14 @@
       </c>
       <c r="B82" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>90</v>
+      </c>
+      <c r="B83" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Estructura de producto en tabla de articulos
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="585" windowWidth="14805" windowHeight="7530"/>
+    <workbookView xWindow="240" yWindow="645" windowWidth="14805" windowHeight="7470"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -658,11 +658,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+  <sheetPr filterMode="1">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,8 +1386,8 @@
       <formula>"terminado"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="84" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
Se implementa estructura de materiales con procedimiento almacenado
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="94">
   <si>
     <t>Tarea</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>acomodar reporte de ordenes de compra saldos cuando se hacen varios ingresos de una misma OC</t>
+  </si>
+  <si>
+    <t>agregar remito interno para descargar stock de piezas facturadas en negro</t>
   </si>
 </sst>
 </file>
@@ -661,10 +664,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,6 +1367,14 @@
       </c>
       <c r="B85" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>93</v>
+      </c>
+      <c r="B86" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modifica reporte de estructura de materiales
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
   <si>
     <t>Tarea</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>agregar remito interno para descargar stock de piezas facturadas en negro</t>
+  </si>
+  <si>
+    <t>reporte retenciones entre fechas</t>
   </si>
 </sst>
 </file>
@@ -664,10 +667,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,6 +1377,14 @@
         <v>93</v>
       </c>
       <c r="B86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reporte de renteciones IIBB
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="96">
   <si>
     <t>Tarea</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>reporte retenciones entre fechas</t>
+  </si>
+  <si>
+    <t>reporte de art comprados sale mal ej oc 129 sintermet en prod</t>
   </si>
 </sst>
 </file>
@@ -667,10 +670,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,6 +1388,14 @@
         <v>94</v>
       </c>
       <c r="B87" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>95</v>
+      </c>
+      <c r="B88" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementacion de proveedores en pedidos internos
Se agrega proveedores sugeridos a los pedidos internos tanto al formulario de pedido como a la grilla de pendientes.
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -682,7 +682,7 @@
   <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,7 +1455,7 @@
   <pageSetup scale="84" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Hoja2!$A$1:$A$3</xm:f>

</xml_diff>

<commit_message>
Cambios estructurales en ingreso de articulos
Se asocia en el detalle de ingreso el detalle de orden de compra
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="645" windowWidth="14805" windowHeight="7470"/>
+    <workbookView xWindow="240" yWindow="705" windowWidth="14805" windowHeight="7410"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
   <si>
     <t>Tarea</t>
   </si>
@@ -316,6 +316,15 @@
   </si>
   <si>
     <t>form clientes ver bus de guardado, no se pintan los campos de gris</t>
+  </si>
+  <si>
+    <t>fix reporte orden de compra calculo de total subtotal e ivas</t>
+  </si>
+  <si>
+    <t>EN REPORTE PEDIDOS AGREGAR COLUMNA DE OT PARA SABER LO QUE ESTA PROGRAMADO</t>
+  </si>
+  <si>
+    <t>EN FORMULARIO DE FACTURA PROVEEDOR NO APARECEN LAS OBSERVACIONES GUARDADAS</t>
   </si>
 </sst>
 </file>
@@ -679,10 +688,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1429,6 +1438,30 @@
         <v>98</v>
       </c>
       <c r="B91" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>99</v>
+      </c>
+      <c r="B92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>100</v>
+      </c>
+      <c r="B93" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>101</v>
+      </c>
+      <c r="B94" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1455,7 +1488,7 @@
   <pageSetup scale="84" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Hoja2!$A$1:$A$3</xm:f>

</xml_diff>

<commit_message>
Reporte compras pendientes fix
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="103">
   <si>
     <t>Tarea</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>EN FORMULARIO DE FACTURA PROVEEDOR NO APARECEN LAS OBSERVACIONES GUARDADAS</t>
+  </si>
+  <si>
+    <t>cotizacion agregar cliente sin dar de alta en tabla</t>
   </si>
 </sst>
 </file>
@@ -688,10 +691,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C94"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,6 +1465,14 @@
         <v>101</v>
       </c>
       <c r="B94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>102</v>
+      </c>
+      <c r="B95" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix ingreso de materiales por orden de compra
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="108">
   <si>
     <t>Tarea</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>agregar en formulario de facturas de proveedores campo para cargar percepciones de iibb en pcia de bs as</t>
+  </si>
+  <si>
+    <t>facturacion, permitir modificar liquidacion de iibb manualmente</t>
+  </si>
+  <si>
+    <t>reporte para saber en que piezas es utilizado un componente</t>
   </si>
 </sst>
 </file>
@@ -700,10 +706,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,7 +1264,7 @@
         <v>74</v>
       </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1418,7 +1424,7 @@
         <v>94</v>
       </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1426,7 +1432,7 @@
         <v>95</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1442,7 +1448,7 @@
         <v>97</v>
       </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1466,7 +1472,7 @@
         <v>100</v>
       </c>
       <c r="B93" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1506,6 +1512,22 @@
         <v>105</v>
       </c>
       <c r="B98" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>106</v>
+      </c>
+      <c r="B99" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>107</v>
+      </c>
+      <c r="B100" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se modifica arquitectura para presentar los reportes
Se comienza con el bundle de articulos
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="705" windowWidth="14805" windowHeight="7410"/>
+    <workbookView xWindow="240" yWindow="765" windowWidth="14805" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$100</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="109">
   <si>
     <t>Tarea</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>reporte para saber en que piezas es utilizado un componente</t>
+  </si>
+  <si>
+    <t>clase para simplificar el servidor de reportes</t>
   </si>
 </sst>
 </file>
@@ -706,10 +709,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -1419,7 +1422,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>94</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>95</v>
       </c>
@@ -1443,7 +1446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -1467,7 +1470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>100</v>
       </c>
@@ -1531,8 +1534,16 @@
         <v>4</v>
       </c>
     </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>108</v>
+      </c>
+      <c r="B101" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C85">
+  <autoFilter ref="A1:C100">
     <filterColumn colId="1">
       <filters>
         <filter val="no comenzado"/>

</xml_diff>

<commit_message>
fix reporte etiquetas de ingreso
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="111">
   <si>
     <t>Tarea</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>ingreso de materiales grilla scrolleable, ver bug grilla para asociar OC</t>
+  </si>
+  <si>
+    <t>ver tema de seguridad y acceso para usuarios no logueados</t>
   </si>
 </sst>
 </file>
@@ -712,7 +715,7 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C99" sqref="C99"/>
@@ -1550,6 +1553,14 @@
         <v>109</v>
       </c>
       <c r="B102" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>110</v>
+      </c>
+      <c r="B103" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Recodeando servidor de reportes
Se terminan reportes de articulos, se agrega hasta el reporte entanqueidad entre fechas y por OT
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="112">
   <si>
     <t>Tarea</t>
   </si>
@@ -352,6 +352,9 @@
   </si>
   <si>
     <t>ver tema de seguridad y acceso para usuarios no logueados</t>
+  </si>
+  <si>
+    <t>implementar plantilla para excepciones no capturadas en el front con los reportes</t>
   </si>
 </sst>
 </file>
@@ -715,10 +718,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1561,6 +1564,14 @@
         <v>110</v>
       </c>
       <c r="B103" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>111</v>
+      </c>
+      <c r="B104" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agrega aviso con numero de remito antes de imprimir
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$104</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -720,8 +720,8 @@
   </sheetPr>
   <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1060,7 @@
         <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1503,12 +1503,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>103</v>
       </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1527,20 +1527,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>106</v>
       </c>
       <c r="B99" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>107</v>
       </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1551,20 +1551,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>109</v>
       </c>
       <c r="B102" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>110</v>
       </c>
       <c r="B103" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,9 +1576,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C100">
+  <autoFilter ref="A1:C104">
     <filterColumn colId="1">
       <filters>
+        <filter val="en proceso"/>
         <filter val="no comenzado"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Edicion de ordenes de compra
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="114">
   <si>
     <t>Tarea</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>implementar plantilla para excepciones no capturadas en el front con los reportes</t>
+  </si>
+  <si>
+    <t>modificacion de oc</t>
+  </si>
+  <si>
+    <t>ot listado arreglar filtro por cliente</t>
   </si>
 </sst>
 </file>
@@ -718,10 +724,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,6 +1578,22 @@
         <v>111</v>
       </c>
       <c r="B104" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>112</v>
+      </c>
+      <c r="B105" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>113</v>
+      </c>
+      <c r="B106" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se corrige overflow de reporte de cobranzas
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
   <si>
     <t>Tarea</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>lista de precios, ver como se manejaran los precios de facturacion a clientes que tienen descuentos</t>
+  </si>
+  <si>
+    <t>orden de compra, cuando inserto el mismo codigo 2 veces no lo reconoce como otra linea en la grilla x mismo id</t>
   </si>
 </sst>
 </file>
@@ -727,10 +730,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,6 +1608,14 @@
         <v>114</v>
       </c>
       <c r="B107" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>115</v>
+      </c>
+      <c r="B108" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix reporte libro IVA compras
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$109</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -736,7 +736,7 @@
   <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,12 +1486,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>99</v>
       </c>
       <c r="B92" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1534,12 +1534,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>105</v>
       </c>
       <c r="B98" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1622,16 +1622,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>116</v>
       </c>
       <c r="B109" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C108">
+  <autoFilter ref="A1:C109">
     <filterColumn colId="1">
       <filters>
         <filter val="en proceso"/>

</xml_diff>

<commit_message>
Reporte movimiento de bancos
Se agrega la relacion con el cliente de la cobranza para vincular el deposito de cheque de terceros
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="118">
   <si>
     <t>Tarea</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>orden de compra, hacer focus en la lupa luego de insertar articulo</t>
+  </si>
+  <si>
+    <t>reporte de mov bancarios, cuando filtro por cheques depositados tiene que traer el nombre del cliente</t>
   </si>
 </sst>
 </file>
@@ -733,10 +736,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,6 +1631,14 @@
       </c>
       <c r="B109" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>117</v>
+      </c>
+      <c r="B110" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ventas controller guardado de factura
Se corrige bug al hacer ND sin IVA se obtenia una division por 0 en el calculo de IIBB
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -738,8 +738,8 @@
   </sheetPr>
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1638,7 +1638,7 @@
         <v>117</v>
       </c>
       <c r="B110" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nueva funcionalidad de hoja de ruta
Permite programar viajes
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="765" windowWidth="14805" windowHeight="7350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="121">
   <si>
     <t>Tarea</t>
   </si>
@@ -373,6 +373,15 @@
   </si>
   <si>
     <t>reporte de mov bancarios, cuando filtro por cheques depositados tiene que traer el nombre del cliente</t>
+  </si>
+  <si>
+    <t>fc 5247 defa, habilitar para facturar cantidades especificas de cada remito</t>
+  </si>
+  <si>
+    <t>citi ventas, desarrollar funcionalidad según sistema NMA</t>
+  </si>
+  <si>
+    <t>implementar funcionalidad de hoja de ruta</t>
   </si>
 </sst>
 </file>
@@ -442,6 +451,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -489,7 +501,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -524,7 +536,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -736,10 +748,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,7 +1578,7 @@
         <v>108</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1639,6 +1651,30 @@
       </c>
       <c r="B110" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>118</v>
+      </c>
+      <c r="B111" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>119</v>
+      </c>
+      <c r="B112" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>120</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificacion de ingreso de OC y creacion de reportes de CITI ventas
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$109</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="123">
   <si>
     <t>Tarea</t>
   </si>
@@ -382,6 +382,12 @@
   </si>
   <si>
     <t>implementar funcionalidad de hoja de ruta</t>
+  </si>
+  <si>
+    <t>ingreso de mat. Compras pendientes con el mismo id problema para seleccionar</t>
+  </si>
+  <si>
+    <t>ordenar viajes de hoja de ruta por pendientes y terminados</t>
   </si>
 </sst>
 </file>
@@ -748,10 +754,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,6 +1681,22 @@
       </c>
       <c r="B113" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>121</v>
+      </c>
+      <c r="B114" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>122</v>
+      </c>
+      <c r="B115" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrega funcionalidad de CITI ventas
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="124">
   <si>
     <t>Tarea</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>ordenar viajes de hoja de ruta por pendientes y terminados</t>
+  </si>
+  <si>
+    <t>agregar reporte de cotizaion a tabla de articulos</t>
   </si>
 </sst>
 </file>
@@ -754,10 +757,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C115"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,7 +1683,7 @@
         <v>120</v>
       </c>
       <c r="B113" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -1688,7 +1691,7 @@
         <v>121</v>
       </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -1696,6 +1699,14 @@
         <v>122</v>
       </c>
       <c r="B115" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>123</v>
+      </c>
+      <c r="B116" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reporte pendientes orden de compra
Se filtran las OC inactivas para que no salgan
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="128">
   <si>
     <t>Tarea</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>cuando llamo a un cliente no trae la posicion de iva el form d cliente</t>
+  </si>
+  <si>
+    <t>cobranzas de clientes, en la grilla de pendientes no mostrar los cbtes que se aplicaron al 100%</t>
   </si>
 </sst>
 </file>
@@ -766,10 +769,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:C120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120"/>
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1740,6 +1743,14 @@
         <v>126</v>
       </c>
       <c r="B119" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>127</v>
+      </c>
+      <c r="B120" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Frontend modificacion de pedidos de clientes
Se limpia el filtro del store antes de cargar los pedidos de clientes
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="130">
   <si>
     <t>Tarea</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>tabla de articulos, agregar boton para ver ots pendientes</t>
+  </si>
+  <si>
+    <t>frontend grilla de modificar pedidos, cuando abro la ventana hay que borrar filtro del store</t>
   </si>
 </sst>
 </file>
@@ -772,10 +775,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,7 +1765,15 @@
         <v>128</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>129</v>
+      </c>
+      <c r="B122" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correccion reporte de libro IVA ventas
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -781,7 +781,7 @@
   <dimension ref="A1:C123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A89" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+      <selection activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1784,7 +1784,7 @@
         <v>130</v>
       </c>
       <c r="B123" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remitos pendientes de facturacion
Se agrega columna frontend con numero de remito en la grilla
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -796,7 +796,7 @@
   <dimension ref="A1:C128"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,7 +1839,7 @@
         <v>135</v>
       </c>
       <c r="B128" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RRHH Liquidacion de sueldos
Cuando se guarda una liquidacion se hace focus nuevamente en el boton de buscar empleado
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$128</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="137">
   <si>
     <t>Tarea</t>
   </si>
@@ -427,6 +427,9 @@
   </si>
   <si>
     <t>fc de proveedores, restriccion para evitar carga duplicada</t>
+  </si>
+  <si>
+    <t>rr liquidacion de sueldos, cuando guardo una liquidacion posicionarse en la lupa de buscar empleado</t>
   </si>
 </sst>
 </file>
@@ -793,10 +796,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C128"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1807,10 +1810,10 @@
         <v>131</v>
       </c>
       <c r="B124" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>132</v>
       </c>
@@ -1818,23 +1821,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>133</v>
       </c>
       <c r="B126" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>134</v>
       </c>
       <c r="B127" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>135</v>
       </c>
@@ -1842,8 +1845,16 @@
         <v>6</v>
       </c>
     </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>136</v>
+      </c>
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C123">
+  <autoFilter ref="A1:C128">
     <filterColumn colId="1">
       <filters>
         <filter val="no comenzado"/>

</xml_diff>

<commit_message>
Validaciones de pedidos de clientes
Se valida cuando se realiza un remito que tiene un pedido asociado.
Si la cantidad entregada del item + la cantidad que se esta remitando
superan la cantidad pedida no se puede confeccionar el remito.
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$130</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="138">
   <si>
     <t>Tarea</t>
   </si>
@@ -430,6 +430,9 @@
   </si>
   <si>
     <t>rr liquidacion de sueldos, cuando guardo una liquidacion posicionarse en la lupa de buscar empleado</t>
+  </si>
+  <si>
+    <t>pedido de clientes, agregar funcionalidad de autorizacion de pedidos para remitar con cantidad autorizada</t>
   </si>
 </sst>
 </file>
@@ -796,10 +799,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C129"/>
+  <dimension ref="A1:C130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1805,7 +1808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>131</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>136</v>
       </c>
@@ -1853,8 +1856,16 @@
         <v>6</v>
       </c>
     </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>137</v>
+      </c>
+      <c r="B130" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C128">
+  <autoFilter ref="A1:C130">
     <filterColumn colId="1">
       <filters>
         <filter val="no comenzado"/>

</xml_diff>

<commit_message>
Historico de compras, no se traen los historicos de OC inactivas
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="142">
   <si>
     <t>Tarea</t>
   </si>
@@ -439,6 +439,12 @@
   </si>
   <si>
     <t>funcionalidad para asociar ot a pedido luego de que la OT fue generada</t>
+  </si>
+  <si>
+    <t>33892 LA ESTRUCTURA DE PRODUCTO ARROJA ERROR</t>
+  </si>
+  <si>
+    <t>ORDEN DE COMPRA, HISTORICO DE COMPRA TRAER ORDENES INACTIVAS</t>
   </si>
 </sst>
 </file>
@@ -805,10 +811,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C132"/>
+  <dimension ref="A1:C134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,6 +1889,22 @@
         <v>139</v>
       </c>
       <c r="B132" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>140</v>
+      </c>
+      <c r="B133" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>141</v>
+      </c>
+      <c r="B134" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se configuran las notificaciones via webSocket segun entorno de trabajo DEV y PROD
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="143">
   <si>
     <t>Tarea</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>ORDEN DE COMPRA, HISTORICO DE COMPRA TRAER ORDENES INACTIVAS</t>
+  </si>
+  <si>
+    <t>separar notificacion del entorno de produccion y desarrollo</t>
   </si>
 </sst>
 </file>
@@ -811,10 +814,10 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C134"/>
+  <dimension ref="A1:C135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,7 +1900,7 @@
         <v>140</v>
       </c>
       <c r="B133" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -1905,6 +1908,14 @@
         <v>141</v>
       </c>
       <c r="B134" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>142</v>
+      </c>
+      <c r="B135" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
RRHH liquidacion de SAC
-Se quita el calculo de antiguedad en la liquidacion de SAC
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$136</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -820,7 +820,7 @@
   <dimension ref="A1:C136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+      <selection activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,7 +1647,7 @@
         <v>108</v>
       </c>
       <c r="B101" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1754,12 +1754,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>122</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1770,12 +1770,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>124</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1882,12 +1882,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>138</v>
       </c>
       <c r="B131" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="132" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
@@ -1922,16 +1922,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>143</v>
       </c>
       <c r="B136" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C135">
+  <autoFilter ref="A1:C136">
     <filterColumn colId="1">
       <filters>
         <filter val="no comenzado"/>

</xml_diff>

<commit_message>
Fix comandos TXT percepciones y retenciones
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -820,7 +820,7 @@
   <dimension ref="A1:C136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B139" sqref="B139"/>
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,7 +1447,7 @@
         <v>83</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Retenciones IIBB correccion del calculo sobre importes netos
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -823,7 +823,7 @@
   <dimension ref="A1:C137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B138" sqref="B138"/>
+      <selection activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,7 +1938,7 @@
         <v>144</v>
       </c>
       <c r="B137" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>